<commit_message>
Modified the template documents
</commit_message>
<xml_diff>
--- a/BalanceSheet/BalanceSheetViewModel/Docs/CurrentJournalTemplate.xlsx
+++ b/BalanceSheet/BalanceSheetViewModel/Docs/CurrentJournalTemplate.xlsx
@@ -15,22 +15,161 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="40">
+  <si>
+    <t>S.No.</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>Debit</t>
+  </si>
+  <si>
+    <t>BaSBIAcc12345678</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>5678 Cr eft ACH</t>
+  </si>
+  <si>
+    <t>Capital</t>
+  </si>
+  <si>
+    <t>IT Refunds 5678 Cr eft ACH</t>
+  </si>
+  <si>
+    <t>Xsalary</t>
+  </si>
+  <si>
+    <t>Professional Tax 5432 Cr ECS Salary</t>
+  </si>
+  <si>
+    <t>XSalaryDedn</t>
+  </si>
+  <si>
+    <t>Transport deduction 5435 Cr ECS Salary</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Conveyance</t>
+  </si>
+  <si>
+    <t>5438 Cr ECS Salary</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>5441 Cr ECS Salary</t>
+  </si>
+  <si>
+    <t>BaCitiAcc98765432</t>
+  </si>
+  <si>
+    <t>5444 Cr ECS Salary</t>
+  </si>
+  <si>
+    <t>Salary TDS 5434 Cr ECS Salary</t>
+  </si>
+  <si>
+    <t>XSalary</t>
+  </si>
+  <si>
+    <t>5439 Cr ECS Salary</t>
+  </si>
+  <si>
+    <t>5442 Cr ECS Salary</t>
+  </si>
+  <si>
+    <t>5445 Cr ECS Salary</t>
+  </si>
+  <si>
+    <t>InvNPS</t>
+  </si>
+  <si>
+    <t>5678 Dr Ins</t>
+  </si>
+  <si>
+    <t>InvPPFSBI</t>
+  </si>
+  <si>
+    <t>Invest</t>
+  </si>
+  <si>
+    <t>XRentHouseSmrithiWA307</t>
+  </si>
+  <si>
+    <t>EquitySharesLarsenAndToubro</t>
+  </si>
+  <si>
+    <t>5678 Cr Ins</t>
+  </si>
+  <si>
+    <t>IncEquitySharesLarsenAndToubro</t>
+  </si>
+  <si>
+    <t>Interest</t>
+  </si>
+  <si>
+    <t>PPF Cr Int</t>
+  </si>
+  <si>
+    <t>IncIntPPF</t>
+  </si>
+  <si>
+    <t>ss</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd\-mmm\-yy"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00008B"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -45,8 +184,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -341,12 +484,735 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="14.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>42572</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>42572</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="4">
+        <v>3000</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>42614</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>42614</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>42614</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1600</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>42614</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="4">
+        <v>30000</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>42614</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>29900</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>42614</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>42644</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>42644</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>42644</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1600</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>42644</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="4">
+        <v>30000</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>42644</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>29900</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>42644</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>42744</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>42744</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="4">
+        <v>15000</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3">
+        <v>42745</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3">
+        <v>42745</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="4">
+        <v>10000</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3">
+        <v>42771</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3">
+        <v>42771</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="4">
+        <v>6000</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3">
+        <v>42776</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3">
+        <v>42776</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="4">
+        <v>10000</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3">
+        <v>42797</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0</v>
+      </c>
+      <c r="G24" s="4">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3">
+        <v>42797</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="4">
+        <v>6000</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3">
+        <v>42819</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" s="4">
+        <v>172181.05</v>
+      </c>
+      <c r="G26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3">
+        <v>42819</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" s="4">
+        <v>50023</v>
+      </c>
+      <c r="G27" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3">
+        <v>42819</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="4">
+        <v>0</v>
+      </c>
+      <c r="G28" s="4">
+        <v>222204.05</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3">
+        <v>42825</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0</v>
+      </c>
+      <c r="G29" s="4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3">
+        <v>42825</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="4">
+        <v>10000</v>
+      </c>
+      <c r="G30" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3">
+        <v>42825</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="4">
+        <v>32</v>
+      </c>
+      <c r="G31" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
Cleaned up the balance sheet
</commit_message>
<xml_diff>
--- a/BalanceSheet/BalanceSheetViewModel/Docs/CurrentJournalTemplate.xlsx
+++ b/BalanceSheet/BalanceSheetViewModel/Docs/CurrentJournalTemplate.xlsx
@@ -485,7 +485,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -536,9 +536,7 @@
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
+      <c r="F2" s="4"/>
       <c r="G2" s="4">
         <v>3000</v>
       </c>
@@ -562,9 +560,7 @@
       <c r="F3" s="4">
         <v>3000</v>
       </c>
-      <c r="G3" s="4">
-        <v>0</v>
-      </c>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2">
@@ -582,9 +578,7 @@
       <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
+      <c r="F4" s="4"/>
       <c r="G4" s="4">
         <v>200</v>
       </c>
@@ -605,9 +599,7 @@
       <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
+      <c r="F5" s="4"/>
       <c r="G5" s="4">
         <v>500</v>
       </c>
@@ -631,9 +623,7 @@
       <c r="F6" s="4">
         <v>1600</v>
       </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2">
@@ -654,9 +644,7 @@
       <c r="F7" s="4">
         <v>30000</v>
       </c>
-      <c r="G7" s="4">
-        <v>0</v>
-      </c>
+      <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="2">
@@ -674,9 +662,7 @@
       <c r="E8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="4">
-        <v>0</v>
-      </c>
+      <c r="F8" s="4"/>
       <c r="G8" s="4">
         <v>29900</v>
       </c>
@@ -697,9 +683,7 @@
       <c r="E9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="4">
-        <v>0</v>
-      </c>
+      <c r="F9" s="4"/>
       <c r="G9" s="4">
         <v>1000</v>
       </c>
@@ -720,9 +704,7 @@
       <c r="E10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="4">
-        <v>0</v>
-      </c>
+      <c r="F10" s="4"/>
       <c r="G10" s="4">
         <v>200</v>
       </c>
@@ -743,9 +725,7 @@
       <c r="E11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="4">
-        <v>0</v>
-      </c>
+      <c r="F11" s="4"/>
       <c r="G11" s="4">
         <v>500</v>
       </c>
@@ -769,9 +749,7 @@
       <c r="F12" s="4">
         <v>1600</v>
       </c>
-      <c r="G12" s="4">
-        <v>0</v>
-      </c>
+      <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2">
@@ -792,9 +770,7 @@
       <c r="F13" s="4">
         <v>30000</v>
       </c>
-      <c r="G13" s="4">
-        <v>0</v>
-      </c>
+      <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2">
@@ -812,9 +788,7 @@
       <c r="E14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="4">
-        <v>0</v>
-      </c>
+      <c r="F14" s="4"/>
       <c r="G14" s="4">
         <v>29900</v>
       </c>
@@ -835,9 +809,7 @@
       <c r="E15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="4">
-        <v>0</v>
-      </c>
+      <c r="F15" s="4"/>
       <c r="G15" s="4">
         <v>1000</v>
       </c>
@@ -858,9 +830,7 @@
       <c r="E16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="4">
-        <v>0</v>
-      </c>
+      <c r="F16" s="4"/>
       <c r="G16" s="4">
         <v>15000</v>
       </c>
@@ -884,9 +854,7 @@
       <c r="F17" s="4">
         <v>15000</v>
       </c>
-      <c r="G17" s="4">
-        <v>0</v>
-      </c>
+      <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2">
@@ -904,9 +872,7 @@
       <c r="E18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="4">
-        <v>0</v>
-      </c>
+      <c r="F18" s="4"/>
       <c r="G18" s="4">
         <v>10000</v>
       </c>
@@ -930,9 +896,7 @@
       <c r="F19" s="4">
         <v>10000</v>
       </c>
-      <c r="G19" s="4">
-        <v>0</v>
-      </c>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="2">
@@ -950,9 +914,7 @@
       <c r="E20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="4">
-        <v>0</v>
-      </c>
+      <c r="F20" s="4"/>
       <c r="G20" s="4">
         <v>6000</v>
       </c>
@@ -976,9 +938,7 @@
       <c r="F21" s="4">
         <v>6000</v>
       </c>
-      <c r="G21" s="4">
-        <v>0</v>
-      </c>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="2">
@@ -996,9 +956,7 @@
       <c r="E22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="4">
-        <v>0</v>
-      </c>
+      <c r="F22" s="4"/>
       <c r="G22" s="4">
         <v>10000</v>
       </c>
@@ -1022,9 +980,7 @@
       <c r="F23" s="4">
         <v>10000</v>
       </c>
-      <c r="G23" s="4">
-        <v>0</v>
-      </c>
+      <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2">
@@ -1042,9 +998,7 @@
       <c r="E24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="4">
-        <v>0</v>
-      </c>
+      <c r="F24" s="4"/>
       <c r="G24" s="4">
         <v>6000</v>
       </c>
@@ -1068,9 +1022,7 @@
       <c r="F25" s="4">
         <v>6000</v>
       </c>
-      <c r="G25" s="4">
-        <v>0</v>
-      </c>
+      <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="2">
@@ -1091,9 +1043,7 @@
       <c r="F26" s="4">
         <v>172181.05</v>
       </c>
-      <c r="G26" s="4">
-        <v>0</v>
-      </c>
+      <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="2">
@@ -1114,9 +1064,7 @@
       <c r="F27" s="4">
         <v>50023</v>
       </c>
-      <c r="G27" s="4">
-        <v>0</v>
-      </c>
+      <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="2">
@@ -1134,9 +1082,7 @@
       <c r="E28" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F28" s="4">
-        <v>0</v>
-      </c>
+      <c r="F28" s="4"/>
       <c r="G28" s="4">
         <v>222204.05</v>
       </c>
@@ -1157,9 +1103,7 @@
       <c r="E29" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F29" s="4">
-        <v>0</v>
-      </c>
+      <c r="F29" s="4"/>
       <c r="G29" s="4">
         <v>10000</v>
       </c>
@@ -1183,9 +1127,7 @@
       <c r="F30" s="4">
         <v>10000</v>
       </c>
-      <c r="G30" s="4">
-        <v>0</v>
-      </c>
+      <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="2">
@@ -1206,9 +1148,7 @@
       <c r="F31" s="4">
         <v>32</v>
       </c>
-      <c r="G31" s="4">
-        <v>0</v>
-      </c>
+      <c r="G31" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>